<commit_message>
Update: dynamic form, robust pipeline, requirements.txt, .gitignore for deployment
</commit_message>
<xml_diff>
--- a/OCC_FOB_predictions.xlsx
+++ b/OCC_FOB_predictions.xlsx
@@ -447,66 +447,66 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>155</v>
+        <v>230</v>
       </c>
       <c r="B2" t="n">
-        <v>121.6543273925781</v>
+        <v>189.35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>185</v>
+        <v>110</v>
       </c>
       <c r="B3" t="n">
-        <v>143.5188751220703</v>
+        <v>100.25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B4" t="n">
-        <v>157.127685546875</v>
+        <v>149.95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B5" t="n">
-        <v>89.75483703613281</v>
+        <v>104.35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="B6" t="n">
-        <v>75.9796142578125</v>
+        <v>143.18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="B7" t="n">
-        <v>237.0178833007812</v>
+        <v>150.66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>120</v>
+        <v>215</v>
       </c>
       <c r="B8" t="n">
-        <v>140.627197265625</v>
+        <v>174.21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="B9" t="n">
-        <v>123.6624374389648</v>
+        <v>125.99</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>169</v>
       </c>
       <c r="B10" t="n">
-        <v>141.4349670410156</v>
+        <v>156.13</v>
       </c>
     </row>
     <row r="11">
@@ -522,23 +522,23 @@
         <v>179</v>
       </c>
       <c r="B11" t="n">
-        <v>185.3752288818359</v>
+        <v>195.43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B12" t="n">
-        <v>134.4204864501953</v>
+        <v>66.95</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B13" t="n">
-        <v>101.1898193359375</v>
+        <v>114.68</v>
       </c>
     </row>
     <row r="14">
@@ -546,23 +546,23 @@
         <v>125</v>
       </c>
       <c r="B14" t="n">
-        <v>128.0927429199219</v>
+        <v>132.56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B15" t="n">
-        <v>95.09912109375</v>
+        <v>112.65</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>180</v>
+        <v>115</v>
       </c>
       <c r="B16" t="n">
-        <v>144.5163879394531</v>
+        <v>131.39</v>
       </c>
     </row>
     <row r="17">
@@ -570,39 +570,39 @@
         <v>193</v>
       </c>
       <c r="B17" t="n">
-        <v>166.1079711914062</v>
+        <v>182.13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B18" t="n">
-        <v>117.1736450195312</v>
+        <v>112.76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="B19" t="n">
-        <v>119.723876953125</v>
+        <v>184.8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="B20" t="n">
-        <v>142.2840881347656</v>
+        <v>159.52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="B21" t="n">
-        <v>108.6879348754883</v>
+        <v>112.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>